<commit_message>
continuação do script na noite de 27-07-2023
</commit_message>
<xml_diff>
--- a/Numeros_Whats.xlsx
+++ b/Numeros_Whats.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renan\Desktop\py\repetidor whats - kaio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\bot whatsapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B210E4-D0A3-4921-9059-C7BE9309F3BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4B0861-9779-4B87-90D0-71E9E015E4C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{B99AC83E-2658-4BDB-9739-B20F0D8ABC59}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="14">
   <si>
     <t>Nome</t>
   </si>
@@ -73,7 +73,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +91,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,13 +162,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C3FAE0-4FE9-41D3-9A19-F4DD6E55BB83}">
-  <dimension ref="A7:F11"/>
+  <dimension ref="A7:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36:XFD62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -654,6 +663,1077 @@
         <v>13</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12">
+        <v>31999999999</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="str">
+        <f>CONCATENATE("Olá ",A12,", ",E12)</f>
+        <v>Olá Renan, Mensagem inicial 1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13">
+        <v>31999999999</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" ref="D13:D14" si="1">CONCATENATE("Olá ",A13,", ",E13)</f>
+        <v>Olá Renan, Mensagem inicial 2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14">
+        <v>31999999999</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>Olá Renan, Mensagem inicial 3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>31999999999</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="str">
+        <f>CONCATENATE("Olá ",A15,", ",E15)</f>
+        <v>Olá Renan, Mensagem inicial 1</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <v>31999999999</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" ref="D16:D17" si="2">CONCATENATE("Olá ",A16,", ",E16)</f>
+        <v>Olá Renan, Mensagem inicial 2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>31999999999</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="str">
+        <f t="shared" si="2"/>
+        <v>Olá Renan, Mensagem inicial 3</v>
+      </c>
+      <c r="E17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>31999999999</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="str">
+        <f>CONCATENATE("Olá ",A18,", ",E18)</f>
+        <v>Olá Renan, Mensagem inicial 1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>31999999999</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" ref="D19:D20" si="3">CONCATENATE("Olá ",A19,", ",E19)</f>
+        <v>Olá Renan, Mensagem inicial 2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>31999999999</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="3"/>
+        <v>Olá Renan, Mensagem inicial 3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>31999999999</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" t="str">
+        <f>CONCATENATE("Olá ",A21,", ",E21)</f>
+        <v>Olá Renan, Mensagem inicial 1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>31999999999</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" ref="D22:D23" si="4">CONCATENATE("Olá ",A22,", ",E22)</f>
+        <v>Olá Renan, Mensagem inicial 2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>31999999999</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="4"/>
+        <v>Olá Renan, Mensagem inicial 3</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24">
+        <v>31999999999</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="str">
+        <f>CONCATENATE("Olá ",A24,", ",E24)</f>
+        <v>Olá Renan, Mensagem inicial 1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25">
+        <v>31999999999</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" ref="D25:D26" si="5">CONCATENATE("Olá ",A25,", ",E25)</f>
+        <v>Olá Renan, Mensagem inicial 2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>31999999999</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="5"/>
+        <v>Olá Renan, Mensagem inicial 3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27">
+        <v>31999999999</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="str">
+        <f>CONCATENATE("Olá ",A27,", ",E27)</f>
+        <v>Olá Renan, Mensagem inicial 1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28">
+        <v>31999999999</v>
+      </c>
+      <c r="C28" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" ref="D28:D29" si="6">CONCATENATE("Olá ",A28,", ",E28)</f>
+        <v>Olá Renan, Mensagem inicial 2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>31999999999</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="6"/>
+        <v>Olá Renan, Mensagem inicial 3</v>
+      </c>
+      <c r="E29" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>31999999999</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="str">
+        <f>CONCATENATE("Olá ",A30,", ",E30)</f>
+        <v>Olá Renan, Mensagem inicial 1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>31999999999</v>
+      </c>
+      <c r="C31" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" ref="D31:D32" si="7">CONCATENATE("Olá ",A31,", ",E31)</f>
+        <v>Olá Renan, Mensagem inicial 2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>31999999999</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="7"/>
+        <v>Olá Renan, Mensagem inicial 3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>31999999999</v>
+      </c>
+      <c r="C33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" t="str">
+        <f>CONCATENATE("Olá ",A33,", ",E33)</f>
+        <v>Olá Renan, Mensagem inicial 1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>31999999999</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" ref="D34:D35" si="8">CONCATENATE("Olá ",A34,", ",E34)</f>
+        <v>Olá Renan, Mensagem inicial 2</v>
+      </c>
+      <c r="E34" t="s">
+        <v>10</v>
+      </c>
+      <c r="F34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>31999999999</v>
+      </c>
+      <c r="C35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="8"/>
+        <v>Olá Renan, Mensagem inicial 3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" s="4" t="str">
+        <f>CONCATENATE("Olá ",A36,", ",E36)</f>
+        <v>Olá Renan, Mensagem inicial 1</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="4" t="str">
+        <f t="shared" ref="D37:D38" si="9">CONCATENATE("Olá ",A37,", ",E37)</f>
+        <v>Olá Renan, Mensagem inicial 2</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="4" t="str">
+        <f t="shared" si="9"/>
+        <v>Olá Renan, Mensagem inicial 3</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="4" t="str">
+        <f>CONCATENATE("Olá ",A39,", ",E39)</f>
+        <v>Olá Renan, Mensagem inicial 1</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B40" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="4" t="str">
+        <f t="shared" ref="D40:D41" si="10">CONCATENATE("Olá ",A40,", ",E40)</f>
+        <v>Olá Renan, Mensagem inicial 2</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="4" t="str">
+        <f t="shared" si="10"/>
+        <v>Olá Renan, Mensagem inicial 3</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="4" t="str">
+        <f>CONCATENATE("Olá ",A42,", ",E42)</f>
+        <v>Olá Renan, Mensagem inicial 1</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="4" t="str">
+        <f t="shared" ref="D43:D44" si="11">CONCATENATE("Olá ",A43,", ",E43)</f>
+        <v>Olá Renan, Mensagem inicial 2</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>Olá Renan, Mensagem inicial 3</v>
+      </c>
+      <c r="E44" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="4" t="str">
+        <f>CONCATENATE("Olá ",A45,", ",E45)</f>
+        <v>Olá Renan, Mensagem inicial 1</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="4" t="str">
+        <f t="shared" ref="D46:D47" si="12">CONCATENATE("Olá ",A46,", ",E46)</f>
+        <v>Olá Renan, Mensagem inicial 2</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="4" t="str">
+        <f t="shared" si="12"/>
+        <v>Olá Renan, Mensagem inicial 3</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="4" t="str">
+        <f>CONCATENATE("Olá ",A48,", ",E48)</f>
+        <v>Olá Renan, Mensagem inicial 1</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="4" t="str">
+        <f t="shared" ref="D49:D50" si="13">CONCATENATE("Olá ",A49,", ",E49)</f>
+        <v>Olá Renan, Mensagem inicial 2</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="4" t="str">
+        <f t="shared" si="13"/>
+        <v>Olá Renan, Mensagem inicial 3</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D51" s="4" t="str">
+        <f>CONCATENATE("Olá ",A51,", ",E51)</f>
+        <v>Olá Renan, Mensagem inicial 1</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="4" t="str">
+        <f t="shared" ref="D52:D53" si="14">CONCATENATE("Olá ",A52,", ",E52)</f>
+        <v>Olá Renan, Mensagem inicial 2</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B53" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="4" t="str">
+        <f t="shared" si="14"/>
+        <v>Olá Renan, Mensagem inicial 3</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B54" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="4" t="str">
+        <f>CONCATENATE("Olá ",A54,", ",E54)</f>
+        <v>Olá Renan, Mensagem inicial 1</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="4" t="str">
+        <f t="shared" ref="D55:D56" si="15">CONCATENATE("Olá ",A55,", ",E55)</f>
+        <v>Olá Renan, Mensagem inicial 2</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B56" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="4" t="str">
+        <f t="shared" si="15"/>
+        <v>Olá Renan, Mensagem inicial 3</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B57" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D57" s="4" t="str">
+        <f>CONCATENATE("Olá ",A57,", ",E57)</f>
+        <v>Olá Renan, Mensagem inicial 1</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B58" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="4" t="str">
+        <f t="shared" ref="D58:D59" si="16">CONCATENATE("Olá ",A58,", ",E58)</f>
+        <v>Olá Renan, Mensagem inicial 2</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B59" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="4" t="str">
+        <f t="shared" si="16"/>
+        <v>Olá Renan, Mensagem inicial 3</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B60" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="4" t="str">
+        <f>CONCATENATE("Olá ",A60,", ",E60)</f>
+        <v>Olá Renan, Mensagem inicial 1</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B61" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="4" t="str">
+        <f t="shared" ref="D61:D62" si="17">CONCATENATE("Olá ",A61,", ",E61)</f>
+        <v>Olá Renan, Mensagem inicial 2</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="4">
+        <v>31999999999</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="4" t="str">
+        <f t="shared" si="17"/>
+        <v>Olá Renan, Mensagem inicial 3</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
versão instavel pronta para testar
</commit_message>
<xml_diff>
--- a/Numeros_Whats.xlsx
+++ b/Numeros_Whats.xlsx
@@ -5,38 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\bot_whatsapp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\bot whatsapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6C39AA-6EAF-456D-8CED-0122266E598C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FC85C4-D5E2-4BC4-9D02-0D4E0359604A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{B99AC83E-2658-4BDB-9739-B20F0D8ABC59}"/>
+    <workbookView xWindow="18285" yWindow="255" windowWidth="20220" windowHeight="13410" xr2:uid="{B99AC83E-2658-4BDB-9739-B20F0D8ABC59}"/>
   </bookViews>
   <sheets>
     <sheet name="WhatsApp" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Nome</t>
   </si>
@@ -53,12 +42,6 @@
     <t>Mensagem Final</t>
   </si>
   <si>
-    <t>Renan</t>
-  </si>
-  <si>
-    <t>C:\Users\renan\OneDrive - PATRIMAR ENGENHARIA S A\Área de Trabalho\py\repetidor whats - kaio\11111.png</t>
-  </si>
-  <si>
     <t>Mensagem</t>
   </si>
   <si>
@@ -68,16 +51,7 @@
     <t>Mensagem Final 1</t>
   </si>
   <si>
-    <t>Mensagem inicial 2</t>
-  </si>
-  <si>
-    <t>Mensagem Final 2</t>
-  </si>
-  <si>
-    <t>Mensagem inicial 3</t>
-  </si>
-  <si>
-    <t>Mensagem Final 3</t>
+    <t>C:\Projetos\bot whatsapp\test.jpg</t>
   </si>
 </sst>
 </file>
@@ -541,7 +515,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29C3FAE0-4FE9-41D3-9A19-F4DD6E55BB83}">
-  <dimension ref="A7:F12"/>
+  <dimension ref="A7:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
@@ -572,94 +546,28 @@
         <v>3</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
       <c r="B9">
-        <v>31999999999</v>
+        <v>31994773182</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D9" t="str">
         <f>CONCATENATE("Olá ",A9,", ",E9)</f>
-        <v>Olá Renan, Mensagem inicial 1</v>
+        <v>Olá , Mensagem inicial 1</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <v>31999999999</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" t="str">
-        <f t="shared" ref="D10:D11" si="0">CONCATENATE("Olá ",A10,", ",E10)</f>
-        <v>Olá Renan, Mensagem inicial 2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11">
-        <v>3.19999999999999E+21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" t="str">
-        <f t="shared" si="0"/>
-        <v>Olá Renan, Mensagem inicial 3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <v>31999999999</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" t="str">
-        <f>CONCATENATE("Olá ",A12,", ",E12)</f>
-        <v>Olá Renan, Mensagem inicial 1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correção da tela de verificação se logou no whapp
</commit_message>
<xml_diff>
--- a/Numeros_Whats.xlsx
+++ b/Numeros_Whats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\bot_whatsapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D51A20C-0853-4DE0-8420-AB0F3031C340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A2F5C0-04EC-4C5E-8800-BC88D7BF014A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14205" yWindow="1140" windowWidth="22755" windowHeight="14295" xr2:uid="{B99AC83E-2658-4BDB-9739-B20F0D8ABC59}"/>
+    <workbookView xWindow="3735" yWindow="1170" windowWidth="22770" windowHeight="14310" xr2:uid="{B99AC83E-2658-4BDB-9739-B20F0D8ABC59}"/>
   </bookViews>
   <sheets>
     <sheet name="WhatsApp" sheetId="1" r:id="rId1"/>
@@ -474,7 +474,7 @@
   <dimension ref="A7:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
correção: não acahava o bt enviar depois de anexar um arquivo
</commit_message>
<xml_diff>
--- a/Numeros_Whats.xlsx
+++ b/Numeros_Whats.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\bot_whatsapp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\#Prontos\bot_whatsapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A2F5C0-04EC-4C5E-8800-BC88D7BF014A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046125BE-5A80-496B-B4B5-90314B531E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3735" yWindow="1170" windowWidth="22770" windowHeight="14310" xr2:uid="{B99AC83E-2658-4BDB-9739-B20F0D8ABC59}"/>
+    <workbookView xWindow="6240" yWindow="3150" windowWidth="29415" windowHeight="12330" xr2:uid="{B99AC83E-2658-4BDB-9739-B20F0D8ABC59}"/>
   </bookViews>
   <sheets>
     <sheet name="WhatsApp" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
     <t>Mensagem Final 1</t>
   </si>
   <si>
-    <t>C:\Projetos\bot whatsapp\test.jpg</t>
+    <t>R:\#Prontos\bot_whatsapp\test.jpg</t>
   </si>
 </sst>
 </file>
@@ -175,9 +175,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -215,7 +215,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -321,7 +321,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -463,7 +463,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>

</xml_diff>